<commit_message>
Formatted gap analysis excel
</commit_message>
<xml_diff>
--- a/backend/data1.xlsx
+++ b/backend/data1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>Sl No.</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>DSA</t>
+  </si>
+  <si>
+    <t>18CS32</t>
   </si>
   <si>
     <t>SUM = A</t>
@@ -125,15 +131,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,7 +479,7 @@
   <dimension ref="A1:Q8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -590,8 +593,12 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
@@ -636,48 +643,82 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>4</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1">
-        <v>3.2</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1">
-        <v>3.2</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
       <c r="H5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
@@ -689,7 +730,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
@@ -701,129 +742,138 @@
         <v>0</v>
       </c>
       <c r="P5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="1">
-        <v>2</v>
+        <v>81.48148148148148</v>
       </c>
       <c r="E6" s="1">
-        <v>1</v>
+        <v>88.14814814814815</v>
       </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>88.14814814814815</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>96.29629629629629</v>
       </c>
       <c r="H6" s="1">
-        <v>0</v>
+        <v>92.5925925925926</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J6" s="1">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="K6" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>85.18518518518519</v>
       </c>
       <c r="M6" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N6" s="1">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="O6" s="1">
-        <v>2</v>
-      </c>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="P6" s="1">
+        <v>85.18518518518519</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>85.18518518518519</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="1">
-        <v>100</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="E7" s="1">
+        <v>12</v>
       </c>
       <c r="F7" s="1">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1">
-        <v>88.14814814814815</v>
+        <v>13</v>
       </c>
       <c r="H7" s="1">
-        <v>88.14814814814815</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="I7" s="1">
+        <v>14</v>
+      </c>
+      <c r="J7" s="1">
+        <v>14</v>
+      </c>
+      <c r="K7" s="1">
+        <v>14</v>
+      </c>
+      <c r="L7" s="1">
+        <v>12</v>
+      </c>
+      <c r="M7" s="1">
+        <v>14</v>
+      </c>
+      <c r="N7" s="1">
+        <v>14</v>
+      </c>
+      <c r="O7" s="1">
+        <v>14</v>
+      </c>
+      <c r="P7" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="3">
-        <v>12</v>
-      </c>
-      <c r="F8" s="3">
-        <v>12</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>19</v>
-      </c>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:C4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>